<commit_message>
Fix ETA date import issue - Convert Excel serial numbers to readable dates in Customer Capital Work Details
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatanathandwarakanathan/Desktop/CC-Dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kharb\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F998A8EA-EB6C-5548-86E8-A75B23E2BFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFDA32E-CA5F-4D4F-BC0A-0DAE8CB14521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39180" yWindow="1520" windowWidth="27640" windowHeight="16940" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Grab" sheetId="2" r:id="rId1"/>
     <sheet name="RAG" sheetId="1" r:id="rId2"/>
+    <sheet name="GA Insights" sheetId="3" r:id="rId3"/>
+    <sheet name="Finance Automation" sheetId="7" r:id="rId4"/>
+    <sheet name="Datawarehouse" sheetId="6" r:id="rId5"/>
+    <sheet name="HR Automation" sheetId="8" r:id="rId6"/>
+    <sheet name="CX Agentic Framework" sheetId="9" r:id="rId7"/>
+    <sheet name="Integration - Agentic Framework" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,8 +34,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
   <si>
     <t>Description</t>
   </si>
@@ -69,32 +73,401 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Dated Updated</t>
-  </si>
-  <si>
-    <t>The RAG-Service enables users to upload PDF, Word, text, Excel, or PowerPoint documents and query their content for enhanced information retrieval and analysis.</t>
-  </si>
-  <si>
     <t>Provides accurate, context-aware responses to user queries based on document content, facilitating informed decision-making.</t>
   </si>
   <si>
-    <t>Scheduled for Monday, August 11, 2025.</t>
-  </si>
-  <si>
-    <t>Kushal from Customer Capital; Dr. Venkat from Shepardtri.</t>
-  </si>
-  <si>
     <t>Achieves accuracies above 95%, with additional testing required to ensure reliability.</t>
   </si>
   <si>
     <t>Proposal submitted and pending approval.</t>
+  </si>
+  <si>
+    <t>GA dashboards</t>
+  </si>
+  <si>
+    <t>Price Grab</t>
+  </si>
+  <si>
+    <t>The software aggregates and compares prices from Amazon, Flipkart, Croma, and Reliance to optimize pricing strategies for enhanced marketability.</t>
+  </si>
+  <si>
+    <t>Provides real-time price comparisons, competitor pricing trends, and demand fluctuations to inform dynamic pricing decisions.</t>
+  </si>
+  <si>
+    <t>UAT in progress and scheduled to go-live by Aug-20.</t>
+  </si>
+  <si>
+    <t>Date Updated(dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Tentative go live planned for end of August</t>
+  </si>
+  <si>
+    <t>The dashboard gives an insight into user behaviour, customer segmentation, volume based metrics to track sales and margin across various categories, products.</t>
+  </si>
+  <si>
+    <t>The GA dashboards enables users to visualise the different metrics using the GA4 data and transactional data from databases such as MySql and Postgres.</t>
+  </si>
+  <si>
+    <t>CC - Srishti / Uma ; ST - Sakthi / Abhinav</t>
+  </si>
+  <si>
+    <t>Datawarehouse</t>
+  </si>
+  <si>
+    <t>Streamline and consolidate multiple segments and sources of sales and input data for understanding and deriving better sales insights to grow and run business better</t>
+  </si>
+  <si>
+    <t>Setup of pipelines to ingest data from various sources and setup ETL processes to transform the data into a more insight driven format. To assist business to drive more revenue growth</t>
+  </si>
+  <si>
+    <t>CC - Ayesha/Srishti/Uma ; ST - Dr Venkat</t>
+  </si>
+  <si>
+    <t>Proposal submitted on 09/Jun/25
+Still under review with CC team till date</t>
+  </si>
+  <si>
+    <t>Awaiting timelines from CC team</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>The RAG-Service enables users to upload PDF, Word, text, Excel, or PowerPoint documents and query their content for enhanced information retrieval and analysis.
+Intent is to create a virtual agents / service which can be leveraged to support activities like learning, customer support etc to boost employee productivity</t>
+  </si>
+  <si>
+    <t>CC - Kushal, CX - Nishit; ST - Dr Venkat</t>
+  </si>
+  <si>
+    <t>POC - UAT in progress. ETA - 21st Aug</t>
+  </si>
+  <si>
+    <t>Two projects under RAG Service
+1. RAG Service - POC UAT in progress
+2. RAG Service CX - Deployed for POC - UAT, Final scoping under review for CX Support BOT</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. IDFC-Tripstacc - 18/Jun/25
+2. IDFC Shopstacc - Tentative Go Live - 18th Aug
+3. Scheduled Reports - 18/Jun/25
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Other Dashboards</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> - Under internal Review (BOB,ET,BOM) - Tentative End of Aug
+HDFC - KPI's scoping in progress - ETA under discussion</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Dashboard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> - HDFC - KPI's scoping in progress with CC team. Fynd and Payment reports still under finalization with CC
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Transction DB for other staccs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> - Replication cost and approval still under discussion internally by CC team
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">Improvements Done </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> - Bigquery Support added to improve performance of Dashboards to overcome postrgres technical syncing issues
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Potential Risks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> - Website updates will lead to data mapping issues causing incorrect data to be reflected in Dashboards. Potential issue with UI changes impacting GA
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Live Dashboards - 1 (Tripstacc)
+Ready for Go Live - 1 (Shopstacc)
+Under Internal Review - 2 (ET, BOM)
+In UAT - 1 (BOB)
+Requirement Scoping - 1 (HDFC)
+Email Scheduler - Live</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Status - 5 Dashboards 
+1. IDFC-Tripstacc- 18 Filters, 67 KPIs
+2. IDFC-Shopstacc- 17 filters, 56 KPIs
+3. BOB card- 8 filters, 39 KPIs
+4. BOM- 8 filters, 36 KPIs- Internal review in progress
+5. ET- 8 filters, 26 KPIs- Internal review in progress
+HDFC - Intial configuration for GA metrics in progress
+Performance KPI's being finalized by CC team
+Transaction DB syncing - On-hold - Awaiting updates from CC on replication
+</t>
+  </si>
+  <si>
+    <t>No Updates received from CC post submission of proposal</t>
+  </si>
+  <si>
+    <t>Finance Automation</t>
+  </si>
+  <si>
+    <t>Implement automation to capture the various input sources like FYND report, Payment Gateway report, Vendor cost master, Mark up master and provide auto calculations for various reports</t>
+  </si>
+  <si>
+    <t>Automate the calculations being done for HDFC using manual excel macros to maintain vendor cost master, MOP and selling margins to assist in sales and margin reporting and revenue tracking (sales/refunds)</t>
+  </si>
+  <si>
+    <t>Tentative ETA - 22-08-2025</t>
+  </si>
+  <si>
+    <t>CC - Manju, Nishant, Ganesh ; ST - Thawpeek / Abhinav</t>
+  </si>
+  <si>
+    <t>1. Input report layouts still being finalized for FYND and Payment gateway
+2. Input test data for Payables automation still pending with CC team
+3. Change requests coming in on ad-hoc basis as the system is being tested in UAT</t>
+  </si>
+  <si>
+    <t>UAT delivery - 18/Jul/25</t>
+  </si>
+  <si>
+    <t>Reports - 
+1. Integration of FYND, PAYU and Vendor Cost Master completed
+2. MOP master import setup completed - UAT in progress
+3. 4 reports delivered for UAT on 15th July 
+CR received for Filters to be provided on reports and develop export intgerations with Power BI and Looker Studio</t>
+  </si>
+  <si>
+    <t>Provide Agentic support for L1 screening and parsing of resume to help shortlist interview candidates for recruitment</t>
+  </si>
+  <si>
+    <t>Agent to provide facility to generate Job Descriptions for various roles and implement a mathematical model to calculate the profile fitment score against the job posting</t>
+  </si>
+  <si>
+    <t>CC - Kunal/Sourabh Kala ; ST - Dr Venkat</t>
+  </si>
+  <si>
+    <t>POC instance setup in progress ETA - 15th Aug</t>
+  </si>
+  <si>
+    <t>Procurement of requisite infra in progress</t>
+  </si>
+  <si>
+    <t>CX Agentic Framework</t>
+  </si>
+  <si>
+    <t>Boost productivity for CX Agents on ground by having customer CRM data accessible easily and faster</t>
+  </si>
+  <si>
+    <t>Provide an integrated UI to the CX Agent on ground to simplify the way to identify the originating customer and retrieve their respective transactional data without searching across multiple portals</t>
+  </si>
+  <si>
+    <t>CC - Nishit Gandhi ; ST - Deva / Abhinav</t>
+  </si>
+  <si>
+    <t>To be finalized once open risks are discussed and closed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">Possible Challenges -
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>1. Would require replication of existing transaction DB's which will incur cost for CC
+2. If DB approach is ruled out then screen scrapping would not be appropriate for accuracy of data capture
+3. Data Security perspective to be reviewed with CC team (Rajeev / Kunal) if agent ID's could be created to export reports on a scheduled basis</t>
+    </r>
+  </si>
+  <si>
+    <t>Initial risk and requirement scoping in progress</t>
+  </si>
+  <si>
+    <t>Initial calls with Rajeev and team to be setup for next week</t>
+  </si>
+  <si>
+    <t>Intgeration -  Agentic Framework</t>
+  </si>
+  <si>
+    <t>Sync ticket information across bank SFDC platform and V-Tiger CRM</t>
+  </si>
+  <si>
+    <t>Provide a way for the CX agent to reconcile and monitor the daily ticket and update summary with bank</t>
+  </si>
+  <si>
+    <t>Initial automation feasibility in progress</t>
+  </si>
+  <si>
+    <t>Proposal to be submitted post initial feasibility check</t>
+  </si>
+  <si>
+    <t>CC - Nishit Gandhi ; ST - Thawpeek / Abhinav</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">Risk - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>SFDC restricts agents to scrape data from screen due to unaidentifiable tags. Ticket classification being done by bank and in V-tiger is different and may need NLP for category corelation</t>
+    </r>
+  </si>
+  <si>
+    <t>4 Portals to be incorporated under price Grab
+Amazon - Deployed - Live 
+Flipkart - Under Internal testing
+Croma / Reliance - Awaiting Input files from CC</t>
+  </si>
+  <si>
+    <t>CC - Nishant Bhagaya / Ganesh; ST - Dr Venkat</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Overcomes Amazon's bot detection algorithms using IP rotation and CAPTCHA-solving techniques to discreetly scrape prices.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Outstanding Items - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Input files awaited from CC(Ganesh) for remaining portals.</t>
+    </r>
+  </si>
+  <si>
+    <t>feasibility under progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -117,7 +490,8 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Display"/>
       <scheme val="major"/>
@@ -127,6 +501,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
       <scheme val="major"/>
     </font>
   </fonts>
@@ -165,24 +547,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,19 +921,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D55975-AAC5-1E49-92F9-E2E68D0D9450}">
-  <dimension ref="B1:C9"/>
+  <dimension ref="B1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6875" customWidth="1"/>
     <col min="3" max="3" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -538,53 +941,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="C3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="C6" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="78.75" x14ac:dyDescent="0.5">
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="2:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="C7" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="7"/>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="63" x14ac:dyDescent="0.5">
+      <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="11">
+        <v>45816</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -593,27 +1020,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4142D79-2110-C948-95C9-B0989E70E4DD}">
-  <dimension ref="B1:C9"/>
+  <dimension ref="B1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="2" max="2" width="28.125" customWidth="1"/>
     <col min="3" max="3" width="62" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -621,60 +1048,644 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" ht="110.25" x14ac:dyDescent="0.5">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="57" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C5" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="38" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C8" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="63" x14ac:dyDescent="0.5">
+      <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="12">
+        <v>45816</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84D2C17-A878-412C-9D99-FA4AA6DB90DE}">
+  <dimension ref="B1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="33.75" customWidth="1"/>
+    <col min="3" max="3" width="69.6875" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="110.25" x14ac:dyDescent="0.5">
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="204.75" x14ac:dyDescent="0.5">
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="94.5" x14ac:dyDescent="0.5">
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="189" x14ac:dyDescent="0.5">
       <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="7">
-        <v>45874</v>
+        <v>29</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.5">
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7">
+        <v>45816</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FB064B-4BFC-4269-9F83-0230D7DE161E}">
+  <dimension ref="C1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="59.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="78.75" x14ac:dyDescent="0.5">
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="110.25" x14ac:dyDescent="0.5">
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="11">
+        <v>45816</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B433B3BE-E625-4D08-B0CE-E95CECD3E1A7}">
+  <dimension ref="C1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="26.75" customWidth="1"/>
+    <col min="4" max="4" width="54.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="11">
+        <v>45816</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920EC9AC-68BC-433F-90F8-95EC7B80EA35}">
+  <dimension ref="C1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
+    <col min="4" max="4" width="56.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="11">
+        <v>45816</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64071BAA-F40B-481F-99E4-B3F4D3E66238}">
+  <dimension ref="C1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
+    <col min="4" max="4" width="56.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="126" x14ac:dyDescent="0.5">
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="11">
+        <v>45816</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D1FD0F-F19C-4797-8962-45DDF1973399}">
+  <dimension ref="C1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="18.25" customWidth="1"/>
+    <col min="4" max="4" width="56.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.5">
+      <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="11">
+        <v>45816</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update shared data - 2025-08-07T01-44-35-073Z
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kharb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatanathandwarakanathan/Desktop/CC-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFDA32E-CA5F-4D4F-BC0A-0DAE8CB14521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CE77DA-48B0-7845-88DE-2E2A1296BEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12980" firstSheet="2" activeTab="7" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Grab" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="75">
   <si>
     <t>Description</t>
   </si>
@@ -348,9 +348,6 @@
     <t>CC - Nishit Gandhi ; ST - Deva / Abhinav</t>
   </si>
   <si>
-    <t>To be finalized once open risks are discussed and closed</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -462,12 +459,27 @@
   <si>
     <t>feasibility under progress</t>
   </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAT </t>
+  </si>
+  <si>
+    <t>Last week of Augus 2025</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -511,6 +523,13 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -520,7 +539,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -543,11 +562,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -587,6 +617,20 @@
     <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,19 +965,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D55975-AAC5-1E49-92F9-E2E68D0D9450}">
-  <dimension ref="B1:C10"/>
+  <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.6875" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="3" max="3" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -941,7 +985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -949,7 +993,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -957,7 +1001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
@@ -965,7 +1009,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
@@ -973,23 +1017,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="78.75" x14ac:dyDescent="0.5">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="102" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.5">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
@@ -997,20 +1041,36 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="63" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:3" ht="68" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="11">
         <v>45816</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1020,19 +1080,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4142D79-2110-C948-95C9-B0989E70E4DD}">
-  <dimension ref="B1:C10"/>
+  <dimension ref="B1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
     <col min="3" max="3" width="62" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1048,7 +1108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="110.25" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:3" ht="112" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1056,7 +1116,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1064,7 +1124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1072,7 +1132,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1080,7 +1140,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1088,7 +1148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1096,7 +1156,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="63" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:3" ht="64" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
@@ -1104,12 +1164,28 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="12">
         <v>45816</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1119,19 +1195,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84D2C17-A878-412C-9D99-FA4AA6DB90DE}">
-  <dimension ref="B1:C10"/>
+  <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.75" customWidth="1"/>
-    <col min="3" max="3" width="69.6875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="69.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1147,7 +1223,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1155,7 +1231,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1163,7 +1239,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="110.25" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:3" ht="112" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1171,7 +1247,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1179,7 +1255,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="204.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:3" ht="208" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1187,7 +1263,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="94.5" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:3" ht="96" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1195,7 +1271,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="189" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:3" ht="192" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>29</v>
       </c>
@@ -1203,12 +1279,28 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="7">
         <v>45816</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="19">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1218,19 +1310,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FB064B-4BFC-4269-9F83-0230D7DE161E}">
-  <dimension ref="C1:D10"/>
+  <dimension ref="C1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="59.875" customWidth="1"/>
+    <col min="4" max="4" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1246,7 +1338,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="3" spans="3:4" ht="64" x14ac:dyDescent="0.2">
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1254,7 +1346,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="4" spans="3:4" ht="48" x14ac:dyDescent="0.2">
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1262,7 +1354,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1270,7 +1362,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1370,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="3:4" ht="78.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="3:4" ht="80" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1286,7 +1378,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="3:4" ht="110.25" x14ac:dyDescent="0.5">
+    <row r="8" spans="3:4" ht="112" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>29</v>
       </c>
@@ -1294,7 +1386,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1302,12 +1394,28 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="3:4" ht="17" x14ac:dyDescent="0.2">
       <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="11">
         <v>45816</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C12" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1317,19 +1425,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B433B3BE-E625-4D08-B0CE-E95CECD3E1A7}">
-  <dimension ref="C1:D9"/>
+  <dimension ref="C1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="26.75" customWidth="1"/>
-    <col min="4" max="4" width="54.375" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1337,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1345,7 +1453,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="3" spans="3:4" ht="48" x14ac:dyDescent="0.2">
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1353,7 +1461,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="4" spans="3:4" ht="48" x14ac:dyDescent="0.2">
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1361,7 +1469,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1369,7 +1477,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1377,7 +1485,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
@@ -1385,7 +1493,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="3:4" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="8" spans="3:4" ht="32" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1393,12 +1501,28 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="3:4" ht="17" x14ac:dyDescent="0.2">
       <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="11">
         <v>45816</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C10" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C11" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1408,19 +1532,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920EC9AC-68BC-433F-90F8-95EC7B80EA35}">
-  <dimension ref="C1:D9"/>
+  <dimension ref="C1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.25" customWidth="1"/>
-    <col min="4" max="4" width="56.625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1428,7 +1552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1436,7 +1560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="3" spans="3:4" ht="32" x14ac:dyDescent="0.2">
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1444,7 +1568,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="4" spans="3:4" ht="48" x14ac:dyDescent="0.2">
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1452,7 +1576,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1460,7 +1584,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1468,13 +1592,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1482,12 +1606,28 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="9" spans="3:4" ht="51" x14ac:dyDescent="0.2">
       <c r="C9" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="11">
         <v>45816</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C10" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C11" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1497,19 +1637,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64071BAA-F40B-481F-99E4-B3F4D3E66238}">
-  <dimension ref="C1:D10"/>
+  <dimension ref="C1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.25" customWidth="1"/>
-    <col min="4" max="4" width="56.625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1517,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1525,7 +1665,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="3" spans="3:4" ht="32" x14ac:dyDescent="0.2">
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1533,7 +1673,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+    <row r="4" spans="3:4" ht="64" x14ac:dyDescent="0.2">
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1541,15 +1681,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1557,36 +1697,52 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="3:4" ht="126" x14ac:dyDescent="0.5">
+    <row r="7" spans="3:4" ht="128" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="17" x14ac:dyDescent="0.2">
       <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="51" x14ac:dyDescent="0.2">
       <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="11">
         <v>45816</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1596,19 +1752,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D1FD0F-F19C-4797-8962-45DDF1973399}">
-  <dimension ref="C1:D10"/>
+  <dimension ref="C1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.25" customWidth="1"/>
-    <col min="4" max="4" width="56.625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1616,76 +1772,92 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" ht="32" x14ac:dyDescent="0.2">
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" ht="31.5" x14ac:dyDescent="0.5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="32" x14ac:dyDescent="0.2">
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="48" x14ac:dyDescent="0.2">
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="17" x14ac:dyDescent="0.2">
       <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" ht="47.25" x14ac:dyDescent="0.5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="51" x14ac:dyDescent="0.2">
       <c r="C10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="11">
         <v>45816</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C12" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update shared data - 2025-08-07T01-59-12-009Z
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatanathandwarakanathan/Desktop/CC-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CE77DA-48B0-7845-88DE-2E2A1296BEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B598EFFE-13A0-C444-89A6-66E46FF0856D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12980" firstSheet="2" activeTab="7" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12980" activeTab="5" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Grab" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="76">
   <si>
     <t>Description</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>Development</t>
+  </si>
+  <si>
+    <t>HR Automation</t>
   </si>
 </sst>
 </file>
@@ -617,8 +620,8 @@
     <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -968,7 +971,7 @@
   <dimension ref="B1:C12"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,7 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84D2C17-A878-412C-9D99-FA4AA6DB90DE}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1534,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920EC9AC-68BC-433F-90F8-95EC7B80EA35}">
   <dimension ref="C1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1557,7 +1560,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="32" x14ac:dyDescent="0.2">
@@ -1754,7 +1757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D1FD0F-F19C-4797-8962-45DDF1973399}">
   <dimension ref="C1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update shared data - 2025-08-07T02-24-32-152Z
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatanathandwarakanathan/Desktop/CC-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B598EFFE-13A0-C444-89A6-66E46FF0856D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA24E2B6-1D1E-044C-AFD1-E2E28AAED4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12980" activeTab="5" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12980" firstSheet="2" activeTab="2" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Grab" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
   <si>
     <t>Description</t>
   </si>
@@ -476,6 +476,9 @@
   </si>
   <si>
     <t>HR Automation</t>
+  </si>
+  <si>
+    <t>Implemented and Few KPI are in UAT</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84D2C17-A878-412C-9D99-FA4AA6DB90DE}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1303,7 +1306,7 @@
         <v>71</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1537,7 +1540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920EC9AC-68BC-433F-90F8-95EC7B80EA35}">
   <dimension ref="C1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update shared data - 2025-08-07T02-32-53-361Z
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatanathandwarakanathan/Desktop/CC-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA24E2B6-1D1E-044C-AFD1-E2E28AAED4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E9A45F-7E42-B842-83BC-14C7F5E6630A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12980" firstSheet="2" activeTab="2" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
   </bookViews>
@@ -478,7 +478,7 @@
     <t>HR Automation</t>
   </si>
   <si>
-    <t>Implemented and Few KPI are in UAT</t>
+    <t xml:space="preserve">Implemented </t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Update shared data - 2025-08-07T03-15-54-715Z
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatanathandwarakanathan/Desktop/CC-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E9A45F-7E42-B842-83BC-14C7F5E6630A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973F2A2D-03EC-2442-A796-53D3D1A247FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12980" firstSheet="2" activeTab="2" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
+    <workbookView xWindow="12840" yWindow="2400" windowWidth="21800" windowHeight="12980" firstSheet="2" activeTab="3" xr2:uid="{5882FBEC-0FA1-654F-8426-4FBE4B6B6E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Grab" sheetId="2" r:id="rId1"/>
     <sheet name="RAG" sheetId="1" r:id="rId2"/>
     <sheet name="GA Insights" sheetId="3" r:id="rId3"/>
-    <sheet name="Finance Automation" sheetId="7" r:id="rId4"/>
-    <sheet name="Datawarehouse" sheetId="6" r:id="rId5"/>
-    <sheet name="HR Automation" sheetId="8" r:id="rId6"/>
-    <sheet name="CX Agentic Framework" sheetId="9" r:id="rId7"/>
-    <sheet name="Integration - Agentic Framework" sheetId="10" r:id="rId8"/>
+    <sheet name="dataTalk" sheetId="11" r:id="rId4"/>
+    <sheet name="Finance Automation" sheetId="7" r:id="rId5"/>
+    <sheet name="Datawarehouse" sheetId="6" r:id="rId6"/>
+    <sheet name="HR Automation" sheetId="8" r:id="rId7"/>
+    <sheet name="CX Agentic Framework" sheetId="9" r:id="rId8"/>
+    <sheet name="Integration - Agentic Framework" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="84">
   <si>
     <t>Description</t>
   </si>
@@ -479,6 +480,27 @@
   </si>
   <si>
     <t xml:space="preserve">Implemented </t>
+  </si>
+  <si>
+    <t>dataTalk</t>
+  </si>
+  <si>
+    <t>Natural language data query platform</t>
+  </si>
+  <si>
+    <t>Transform the way your business harnesses data with DataTalk—the ultimate web-based platform that redefines data interaction with blazing-fast AI technology! Say goodbye to complex queries, endless spreadsheets, and data silos. With DataTalk, you hold the key to unlocking actionable insights with unmatched ease, speed, and precision. Whether you're a startup hustling to make waves or an enterprise dominating the market, DataTalk empowers everyone—from analysts to executives—to tap into the full potential of your data like never before.</t>
+  </si>
+  <si>
+    <t>Awaiting timelines from CC team for Testing</t>
+  </si>
+  <si>
+    <t>CC - Srishti/Uma ; ST - Dr Venkat</t>
+  </si>
+  <si>
+    <t>Pending approval</t>
+  </si>
+  <si>
+    <t>PoC</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84D2C17-A878-412C-9D99-FA4AA6DB90DE}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1315,6 +1337,113 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35789B37-4E0E-5B44-8301-FE51FE01643F}">
+  <dimension ref="C1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="54.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="192" x14ac:dyDescent="0.2">
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="11">
+        <v>45816</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C10" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C11" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FB064B-4BFC-4269-9F83-0230D7DE161E}">
   <dimension ref="C1:D12"/>
   <sheetViews>
@@ -1429,12 +1558,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B433B3BE-E625-4D08-B0CE-E95CECD3E1A7}">
   <dimension ref="C1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C1" sqref="C1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1536,7 +1665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920EC9AC-68BC-433F-90F8-95EC7B80EA35}">
   <dimension ref="C1:D11"/>
   <sheetViews>
@@ -1641,7 +1770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64071BAA-F40B-481F-99E4-B3F4D3E66238}">
   <dimension ref="C1:D12"/>
   <sheetViews>
@@ -1756,7 +1885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D1FD0F-F19C-4797-8962-45DDF1973399}">
   <dimension ref="C1:D12"/>
   <sheetViews>

</xml_diff>